<commit_message>
Record the local best instead of the next state.
- As a result, the performance imroved a little.
</commit_message>
<xml_diff>
--- a/HCMCMC/HCMCMC/top10.xlsx
+++ b/HCMCMC/HCMCMC/top10.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>T</t>
   </si>
@@ -42,6 +42,10 @@
   <si>
     <t>Use simulated HC to estimate scores
 （ユーザによる誤差（ユーザ50人））</t>
+  </si>
+  <si>
+    <t>Use true scores (各ステップで最大値をサンプリング）
+（MCMCによる誤差）</t>
   </si>
 </sst>
 </file>
@@ -498,11 +502,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="89072768"/>
-        <c:axId val="60087680"/>
+        <c:axId val="71577984"/>
+        <c:axId val="71579520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="89072768"/>
+        <c:axId val="71577984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -513,12 +517,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60087680"/>
+        <c:crossAx val="71579520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="60087680"/>
+        <c:axId val="71579520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -530,7 +534,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89072768"/>
+        <c:crossAx val="71577984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -589,78 +593,84 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'3次元'!$A$2:$A$11</c:f>
+              <c:f>'3次元'!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>90</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'3次元'!$B$2:$B$11</c:f>
+              <c:f>'3次元'!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.6</c:v>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.26</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8</c:v>
+                  <c:v>0.42</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.9</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.9</c:v>
+                  <c:v>0.82</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.9</c:v>
+                  <c:v>0.89</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0.94</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0.97</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0.98</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>0.98</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -672,7 +682,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'3次元'!$C$1</c:f>
+              <c:f>'3次元'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -684,49 +694,52 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'3次元'!$A$2:$A$11</c:f>
+              <c:f>'3次元'!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>90</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'3次元'!$C$2:$C$11</c:f>
+              <c:f>'3次元'!$D$2:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.5</c:v>
                 </c:pt>
@@ -767,7 +780,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'3次元'!$D$1</c:f>
+              <c:f>'3次元'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -779,49 +792,52 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'3次元'!$A$2:$A$11</c:f>
+              <c:f>'3次元'!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>90</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'3次元'!$D$2:$D$11</c:f>
+              <c:f>'3次元'!$E$2:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.3</c:v>
                 </c:pt>
@@ -862,7 +878,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'3次元'!$E$1</c:f>
+              <c:f>'3次元'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -874,49 +890,52 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'3次元'!$A$2:$A$11</c:f>
+              <c:f>'3次元'!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>90</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'3次元'!$E$2:$E$11</c:f>
+              <c:f>'3次元'!$F$2:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.4</c:v>
                 </c:pt>
@@ -951,7 +970,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'3次元'!$F$1</c:f>
+              <c:f>'3次元'!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -963,50 +982,136 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'3次元'!$A$2:$A$11</c:f>
+              <c:f>'3次元'!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>90</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'3次元'!$F$2:$F$11</c:f>
+              <c:f>'3次元'!$G$2:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="7">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'3次元'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Use true scores (各ステップで最大値をサンプリング）
+（MCMCによる誤差）</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'3次元'!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'3次元'!$C$2:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.9</c:v>
                 </c:pt>
               </c:numCache>
@@ -1022,13 +1127,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="79511552"/>
-        <c:axId val="79509760"/>
+        <c:axId val="71828608"/>
+        <c:axId val="71830144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="79511552"/>
+        <c:axId val="71828608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1036,12 +1142,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79509760"/>
+        <c:crossAx val="71830144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="79509760"/>
+        <c:axId val="71830144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1053,7 +1159,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79511552"/>
+        <c:crossAx val="71828608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1116,14 +1222,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>14286</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>457199</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1435,7 +1541,7 @@
   <dimension ref="A3:F14"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:F14"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1648,18 +1754,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="6" width="21.42578125" customWidth="1"/>
+    <col min="2" max="7" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1667,149 +1773,164 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="B2">
+        <v>0.26</v>
+      </c>
+      <c r="C2">
+        <v>0.63</v>
+      </c>
+      <c r="D2">
+        <v>0.5</v>
+      </c>
+      <c r="E2">
+        <v>0.3</v>
+      </c>
+      <c r="F2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>100</v>
+      </c>
+      <c r="B3">
+        <v>0.42</v>
+      </c>
+      <c r="C3">
+        <v>0.82</v>
+      </c>
+      <c r="D3">
         <v>0.6</v>
-      </c>
-      <c r="C2">
-        <v>0.5</v>
-      </c>
-      <c r="D2">
-        <v>0.3</v>
-      </c>
-      <c r="E2">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>20</v>
-      </c>
-      <c r="B3">
-        <v>0.8</v>
-      </c>
-      <c r="C3">
-        <v>0.6</v>
-      </c>
-      <c r="D3">
-        <v>0.5</v>
       </c>
       <c r="E3">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>30</v>
+        <v>200</v>
       </c>
       <c r="B4">
-        <v>0.9</v>
+        <v>0.65</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0.92</v>
       </c>
       <c r="D4">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>40</v>
+        <v>300</v>
       </c>
       <c r="B5">
-        <v>0.9</v>
+        <v>0.82</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
         <v>0.7</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>50</v>
+        <v>400</v>
       </c>
       <c r="B6">
-        <v>0.9</v>
+        <v>0.89</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="D6">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E6">
+        <v>0.9</v>
+      </c>
+      <c r="F6">
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
+        <v>0.94</v>
       </c>
       <c r="D7">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>70</v>
+        <v>600</v>
       </c>
       <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
+        <v>0.97</v>
       </c>
       <c r="D8">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>80</v>
+        <v>700</v>
       </c>
       <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="D9">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <v>0.9</v>
@@ -1817,33 +1938,44 @@
       <c r="F9">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>90</v>
+        <v>800</v>
       </c>
       <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="D10">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>100</v>
+        <v>900</v>
       </c>
       <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="D11">
-        <v>0.9</v>
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1000</v>
+      </c>
+      <c r="B12">
+        <v>0.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>